<commit_message>
Results for first 3 test added to report and explanations added
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Algorthems and data structures\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Paul\Documents\Uni\Algorithms and Data Structures\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -102,10 +102,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -140,7 +140,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -449,7 +448,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -758,7 +756,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1067,7 +1064,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1376,7 +1372,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1710,7 +1705,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2035,7 +2029,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2406,16 +2399,13 @@
               <a:buFontTx/>
               <a:buNone/>
               <a:tabLst/>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr>
                 <a:solidFill>
                   <a:sysClr val="windowText" lastClr="000000">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:sysClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
@@ -2425,7 +2415,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2764,7 +2753,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3098,7 +3086,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8870,14 +8857,14 @@
     <xdr:from>
       <xdr:col>9</xdr:col>
       <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
       <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8899,15 +8886,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -9245,6 +9232,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9280,6 +9284,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9434,7 +9455,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:I113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H94" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
       <selection activeCell="R113" sqref="R113"/>
     </sheetView>
   </sheetViews>
@@ -9445,29 +9466,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="3:9" s="1" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="2"/>
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="G2" s="2"/>
+      <c r="H2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="3"/>
+      <c r="I2" s="2"/>
     </row>
     <row r="3" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
@@ -9723,127 +9744,127 @@
       </c>
     </row>
     <row r="15" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3" t="s">
+      <c r="E15" s="2"/>
+      <c r="F15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3" t="s">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I15" s="3"/>
+      <c r="I15" s="2"/>
     </row>
     <row r="16" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D16" s="3" t="s">
+      <c r="D16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3" t="s">
+      <c r="E16" s="2"/>
+      <c r="F16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3" t="s">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I16" s="3"/>
+      <c r="I16" s="2"/>
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="str">
         <f>C1</f>
         <v>Ulysses 22</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <f>AVERAGE(D4:D13)</f>
         <v>0</v>
       </c>
-      <c r="E17" s="3"/>
-      <c r="F17" s="3">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2">
         <f>AVERAGE(F4:F13)</f>
         <v>12.4</v>
       </c>
-      <c r="G17" s="3"/>
-      <c r="H17" s="3">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2">
         <f>AVERAGE(H4:H13)</f>
         <v>15.5</v>
       </c>
-      <c r="I17" s="3"/>
+      <c r="I17" s="2"/>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D19" s="3" t="s">
+      <c r="D19" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3" t="s">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G19" s="3"/>
-      <c r="H19" s="3" t="s">
+      <c r="G19" s="2"/>
+      <c r="H19" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I19" s="3"/>
+      <c r="I19" s="2"/>
     </row>
     <row r="20" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D20" s="3" t="s">
+      <c r="D20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3" t="s">
+      <c r="G20" s="2"/>
+      <c r="H20" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I20" s="3"/>
+      <c r="I20" s="2"/>
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" t="str">
         <f>C1</f>
         <v>Ulysses 22</v>
       </c>
-      <c r="D21" s="3">
+      <c r="D21" s="2">
         <f>AVERAGE(E4:E13)</f>
         <v>88.89</v>
       </c>
-      <c r="E21" s="3"/>
-      <c r="F21" s="3">
+      <c r="E21" s="2"/>
+      <c r="F21" s="2">
         <f>AVERAGE(G4:G13)</f>
         <v>82.430449999999993</v>
       </c>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3">
+      <c r="G21" s="2"/>
+      <c r="H21" s="2">
         <f>AVERAGE(I4:I13)</f>
         <v>88.89</v>
       </c>
-      <c r="I21" s="3"/>
+      <c r="I21" s="2"/>
     </row>
     <row r="24" spans="3:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="C24" s="2" t="s">
+      <c r="C24" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3" t="s">
+      <c r="E25" s="2"/>
+      <c r="F25" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3" t="s">
+      <c r="G25" s="2"/>
+      <c r="H25" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I25" s="3"/>
+      <c r="I25" s="2"/>
     </row>
     <row r="26" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
@@ -10099,127 +10120,127 @@
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3" t="s">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3" t="s">
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I38" s="3"/>
+      <c r="I38" s="2"/>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3" t="s">
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3" t="s">
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I39" s="3"/>
+      <c r="I39" s="2"/>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
         <f>C24</f>
         <v>Berlin 52</v>
       </c>
-      <c r="D40" s="3">
+      <c r="D40" s="2">
         <f>AVERAGE(D27:D36)</f>
         <v>10.8</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3">
+      <c r="E40" s="2"/>
+      <c r="F40" s="2">
         <f>AVERAGE(F27:F36)</f>
         <v>18.7</v>
       </c>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3">
+      <c r="G40" s="2"/>
+      <c r="H40" s="2">
         <f>AVERAGE(H27:H36)</f>
         <v>115.7</v>
       </c>
-      <c r="I40" s="3"/>
+      <c r="I40" s="2"/>
     </row>
     <row r="42" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3" t="s">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3" t="s">
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I42" s="3"/>
+      <c r="I42" s="2"/>
     </row>
     <row r="43" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D43" s="3" t="s">
+      <c r="D43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3" t="s">
+      <c r="E43" s="2"/>
+      <c r="F43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3" t="s">
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I43" s="3"/>
+      <c r="I43" s="2"/>
     </row>
     <row r="44" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C44" t="str">
         <f>C24</f>
         <v>Berlin 52</v>
       </c>
-      <c r="D44" s="3">
+      <c r="D44" s="2">
         <f>AVERAGE(E27:E36)</f>
         <v>8905.1279999999988</v>
       </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3">
+      <c r="E44" s="2"/>
+      <c r="F44" s="2">
         <f>AVERAGE(G27:G36)</f>
         <v>8732.3454000000002</v>
       </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3">
+      <c r="G44" s="2"/>
+      <c r="H44" s="2">
         <f>AVERAGE(I27:I36)</f>
         <v>8905.1279999999988</v>
       </c>
-      <c r="I44" s="3"/>
+      <c r="I44" s="2"/>
     </row>
     <row r="47" spans="3:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="C47" s="2" t="s">
+      <c r="C47" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D47" s="2"/>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="2"/>
-      <c r="H47" s="2"/>
-      <c r="I47" s="2"/>
+      <c r="D47" s="3"/>
+      <c r="E47" s="3"/>
+      <c r="F47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="3"/>
+      <c r="I47" s="3"/>
     </row>
     <row r="48" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D48" s="3" t="s">
+      <c r="D48" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E48" s="3"/>
-      <c r="F48" s="3" t="s">
+      <c r="E48" s="2"/>
+      <c r="F48" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G48" s="3"/>
-      <c r="H48" s="3" t="s">
+      <c r="G48" s="2"/>
+      <c r="H48" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I48" s="3"/>
+      <c r="I48" s="2"/>
     </row>
     <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" t="s">
@@ -10475,127 +10496,127 @@
       </c>
     </row>
     <row r="61" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D61" s="3" t="s">
+      <c r="D61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3" t="s">
+      <c r="E61" s="2"/>
+      <c r="F61" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3" t="s">
+      <c r="G61" s="2"/>
+      <c r="H61" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I61" s="3"/>
+      <c r="I61" s="2"/>
     </row>
     <row r="62" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D62" s="3" t="s">
+      <c r="D62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3" t="s">
+      <c r="E62" s="2"/>
+      <c r="F62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3" t="s">
+      <c r="G62" s="2"/>
+      <c r="H62" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I62" s="3"/>
+      <c r="I62" s="2"/>
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
         <f>C47</f>
         <v>pr144</v>
       </c>
-      <c r="D63" s="3">
+      <c r="D63" s="2">
         <f>AVERAGE(D50:D59)</f>
         <v>15.6</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3">
+      <c r="E63" s="2"/>
+      <c r="F63" s="2">
         <f>AVERAGE(F50:F59)</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3">
+      <c r="G63" s="2"/>
+      <c r="H63" s="2">
         <f>AVERAGE(H50:H59)</f>
         <v>4306.3999999999996</v>
       </c>
-      <c r="I63" s="3"/>
+      <c r="I63" s="2"/>
     </row>
     <row r="65" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D65" s="3" t="s">
+      <c r="D65" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3" t="s">
+      <c r="E65" s="2"/>
+      <c r="F65" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3" t="s">
+      <c r="G65" s="2"/>
+      <c r="H65" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I65" s="3"/>
+      <c r="I65" s="2"/>
     </row>
     <row r="66" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D66" s="3" t="s">
+      <c r="D66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3" t="s">
+      <c r="E66" s="2"/>
+      <c r="F66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3" t="s">
+      <c r="G66" s="2"/>
+      <c r="H66" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I66" s="3"/>
+      <c r="I66" s="2"/>
     </row>
     <row r="67" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C67" t="str">
         <f>C47</f>
         <v>pr144</v>
       </c>
-      <c r="D67" s="3">
+      <c r="D67" s="2">
         <f>AVERAGE(E50:E59)</f>
         <v>61401.735000000001</v>
       </c>
-      <c r="E67" s="3"/>
-      <c r="F67" s="3">
+      <c r="E67" s="2"/>
+      <c r="F67" s="2">
         <f>AVERAGE(G50:G59)</f>
         <v>61021.864800000003</v>
       </c>
-      <c r="G67" s="3"/>
-      <c r="H67" s="3">
+      <c r="G67" s="2"/>
+      <c r="H67" s="2">
         <f>AVERAGE(I50:I59)</f>
         <v>61401.735000000001</v>
       </c>
-      <c r="I67" s="3"/>
+      <c r="I67" s="2"/>
     </row>
     <row r="70" spans="3:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="C70" s="2" t="s">
+      <c r="C70" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D70" s="2"/>
-      <c r="E70" s="2"/>
-      <c r="F70" s="2"/>
-      <c r="G70" s="2"/>
-      <c r="H70" s="2"/>
-      <c r="I70" s="2"/>
+      <c r="D70" s="3"/>
+      <c r="E70" s="3"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="3"/>
+      <c r="H70" s="3"/>
+      <c r="I70" s="3"/>
     </row>
     <row r="71" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D71" s="3" t="s">
+      <c r="D71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3" t="s">
+      <c r="E71" s="2"/>
+      <c r="F71" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3" t="s">
+      <c r="G71" s="2"/>
+      <c r="H71" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I71" s="3"/>
+      <c r="I71" s="2"/>
     </row>
     <row r="72" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
@@ -10851,127 +10872,127 @@
       </c>
     </row>
     <row r="84" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D84" s="3" t="s">
+      <c r="D84" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E84" s="3"/>
-      <c r="F84" s="3" t="s">
+      <c r="E84" s="2"/>
+      <c r="F84" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G84" s="3"/>
-      <c r="H84" s="3" t="s">
+      <c r="G84" s="2"/>
+      <c r="H84" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I84" s="3"/>
+      <c r="I84" s="2"/>
     </row>
     <row r="85" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D85" s="3" t="s">
+      <c r="D85" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E85" s="3"/>
-      <c r="F85" s="3" t="s">
+      <c r="E85" s="2"/>
+      <c r="F85" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G85" s="3"/>
-      <c r="H85" s="3" t="s">
+      <c r="G85" s="2"/>
+      <c r="H85" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I85" s="3"/>
+      <c r="I85" s="2"/>
     </row>
     <row r="86" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C86" t="str">
         <f>C70</f>
         <v>a280</v>
       </c>
-      <c r="D86" s="3">
+      <c r="D86" s="2">
         <f>AVERAGE(D73:D82)</f>
         <v>15.6</v>
       </c>
-      <c r="E86" s="3"/>
-      <c r="F86" s="3">
+      <c r="E86" s="2"/>
+      <c r="F86" s="2">
         <f>AVERAGE(F73:F82)</f>
         <v>33</v>
       </c>
-      <c r="G86" s="3"/>
-      <c r="H86" s="3">
+      <c r="G86" s="2"/>
+      <c r="H86" s="2">
         <f>AVERAGE(H73:H82)</f>
         <v>58941</v>
       </c>
-      <c r="I86" s="3"/>
+      <c r="I86" s="2"/>
     </row>
     <row r="88" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D88" s="3" t="s">
+      <c r="D88" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E88" s="3"/>
-      <c r="F88" s="3" t="s">
+      <c r="E88" s="2"/>
+      <c r="F88" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G88" s="3"/>
-      <c r="H88" s="3" t="s">
+      <c r="G88" s="2"/>
+      <c r="H88" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I88" s="3"/>
+      <c r="I88" s="2"/>
     </row>
     <row r="89" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D89" s="3" t="s">
+      <c r="D89" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E89" s="3"/>
-      <c r="F89" s="3" t="s">
+      <c r="E89" s="2"/>
+      <c r="F89" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G89" s="3"/>
-      <c r="H89" s="3" t="s">
+      <c r="G89" s="2"/>
+      <c r="H89" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I89" s="3"/>
+      <c r="I89" s="2"/>
     </row>
     <row r="90" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C90" t="str">
         <f>C70</f>
         <v>a280</v>
       </c>
-      <c r="D90" s="3">
+      <c r="D90" s="2">
         <f>AVERAGE(E73:E82)</f>
         <v>3115.5189999999998</v>
       </c>
-      <c r="E90" s="3"/>
-      <c r="F90" s="3">
+      <c r="E90" s="2"/>
+      <c r="F90" s="2">
         <f>AVERAGE(G73:G82)</f>
         <v>3114.0409</v>
       </c>
-      <c r="G90" s="3"/>
-      <c r="H90" s="3">
+      <c r="G90" s="2"/>
+      <c r="H90" s="2">
         <f>AVERAGE(I73:I82)</f>
         <v>3026.9749999999995</v>
       </c>
-      <c r="I90" s="3"/>
+      <c r="I90" s="2"/>
     </row>
     <row r="93" spans="3:9" ht="33.75" x14ac:dyDescent="0.5">
-      <c r="C93" s="2" t="s">
+      <c r="C93" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D93" s="2"/>
-      <c r="E93" s="2"/>
-      <c r="F93" s="2"/>
-      <c r="G93" s="2"/>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
+      <c r="D93" s="3"/>
+      <c r="E93" s="3"/>
+      <c r="F93" s="3"/>
+      <c r="G93" s="3"/>
+      <c r="H93" s="3"/>
+      <c r="I93" s="3"/>
     </row>
     <row r="94" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D94" s="3" t="s">
+      <c r="D94" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E94" s="3"/>
-      <c r="F94" s="3" t="s">
+      <c r="E94" s="2"/>
+      <c r="F94" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G94" s="3"/>
-      <c r="H94" s="3" t="s">
+      <c r="G94" s="2"/>
+      <c r="H94" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I94" s="3"/>
+      <c r="I94" s="2"/>
     </row>
     <row r="95" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C95" t="s">
@@ -11227,148 +11248,148 @@
       </c>
     </row>
     <row r="107" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D107" s="3" t="s">
+      <c r="D107" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E107" s="3"/>
-      <c r="F107" s="3" t="s">
+      <c r="E107" s="2"/>
+      <c r="F107" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G107" s="3"/>
-      <c r="H107" s="3" t="s">
+      <c r="G107" s="2"/>
+      <c r="H107" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I107" s="3"/>
+      <c r="I107" s="2"/>
     </row>
     <row r="108" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D108" s="3" t="s">
+      <c r="D108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E108" s="3"/>
-      <c r="F108" s="3" t="s">
+      <c r="E108" s="2"/>
+      <c r="F108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G108" s="3"/>
-      <c r="H108" s="3" t="s">
+      <c r="G108" s="2"/>
+      <c r="H108" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I108" s="3"/>
+      <c r="I108" s="2"/>
     </row>
     <row r="109" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C109" t="str">
         <f>C93</f>
         <v>ali535</v>
       </c>
-      <c r="D109" s="3">
+      <c r="D109" s="2">
         <f>AVERAGE(D96:D105)</f>
         <v>16.7</v>
       </c>
-      <c r="E109" s="3"/>
-      <c r="F109" s="3">
+      <c r="E109" s="2"/>
+      <c r="F109" s="2">
         <f>AVERAGE(F96:F105)</f>
         <v>62.3</v>
       </c>
-      <c r="G109" s="3"/>
-      <c r="H109" s="3">
+      <c r="G109" s="2"/>
+      <c r="H109" s="2">
         <f>AVERAGE(H96:H105)</f>
         <v>708026.3</v>
       </c>
-      <c r="I109" s="3"/>
+      <c r="I109" s="2"/>
     </row>
     <row r="111" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D111" s="3" t="s">
+      <c r="D111" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E111" s="3"/>
-      <c r="F111" s="3" t="s">
+      <c r="E111" s="2"/>
+      <c r="F111" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="G111" s="3"/>
-      <c r="H111" s="3" t="s">
+      <c r="G111" s="2"/>
+      <c r="H111" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="I111" s="3"/>
+      <c r="I111" s="2"/>
     </row>
     <row r="112" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="D112" s="3" t="s">
+      <c r="D112" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E112" s="3"/>
-      <c r="F112" s="3" t="s">
+      <c r="E112" s="2"/>
+      <c r="F112" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G112" s="3"/>
-      <c r="H112" s="3" t="s">
+      <c r="G112" s="2"/>
+      <c r="H112" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I112" s="3"/>
+      <c r="I112" s="2"/>
     </row>
     <row r="113" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C113" t="str">
         <f>C93</f>
         <v>ali535</v>
       </c>
-      <c r="D113" s="3">
+      <c r="D113" s="2">
         <f>AVERAGE(E96:E105)</f>
         <v>2670.2469999999998</v>
       </c>
-      <c r="E113" s="3"/>
-      <c r="F113" s="3">
+      <c r="E113" s="2"/>
+      <c r="F113" s="2">
         <f>AVERAGE(G96:G105)</f>
         <v>2593.8627999999999</v>
       </c>
-      <c r="G113" s="3"/>
-      <c r="H113" s="3">
+      <c r="G113" s="2"/>
+      <c r="H113" s="2">
         <f>AVERAGE(I96:I105)</f>
         <v>2524.7743999999993</v>
       </c>
-      <c r="I113" s="3"/>
+      <c r="I113" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="110">
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
-    <mergeCell ref="D90:E90"/>
-    <mergeCell ref="F90:G90"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="D62:E62"/>
-    <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C93:I93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="F109:G109"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="D85:E85"/>
     <mergeCell ref="D113:E113"/>
     <mergeCell ref="F113:G113"/>
     <mergeCell ref="F112:G112"/>
@@ -11393,49 +11414,49 @@
     <mergeCell ref="H107:I107"/>
     <mergeCell ref="F107:G107"/>
     <mergeCell ref="D107:E107"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="F109:G109"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="D85:E85"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C93:I93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:G86"/>
+    <mergeCell ref="D90:E90"/>
+    <mergeCell ref="F90:G90"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="D62:E62"/>
+    <mergeCell ref="F62:G62"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Completed results section of report
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Users\Paul\Documents\Uni\Algorithms and Data Structures\Coursework\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Algorthems and data structures\Coursework\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="16">
   <si>
     <t>Run</t>
   </si>
@@ -57,6 +57,21 @@
   </si>
   <si>
     <t>ali535</t>
+  </si>
+  <si>
+    <t>22 Point</t>
+  </si>
+  <si>
+    <t>52 Point</t>
+  </si>
+  <si>
+    <t>144 Point</t>
+  </si>
+  <si>
+    <t>280 Point</t>
+  </si>
+  <si>
+    <t>535 Point</t>
   </si>
 </sst>
 </file>
@@ -140,6 +155,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -448,6 +464,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -741,6 +758,1179 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Time</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> for Different Point Sizes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$D$115:$D$116</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Nearest Neighbour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$117:$C$121</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22 Point</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52 Point</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144 Point</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280 Point</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$117:$D$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>10.8</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.6</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>16.7</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-26D6-4211-8B4D-CFFC194212BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$F$115:$F$116</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Random Nearest Neighbour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$117:$C$121</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22 Point</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52 Point</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144 Point</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280 Point</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$F$117:$F$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>12.4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>17.399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>62.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-26D6-4211-8B4D-CFFC194212BC}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="365130440"/>
+        <c:axId val="365946360"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$115:$E$116</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Nearest Neighbour</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Time</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$117:$C$121</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>22 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>52 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>144 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>280 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>535 Point</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$E$117:$E$121</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-26D6-4211-8B4D-CFFC194212BC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="3"/>
+                <c:order val="3"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$115:$G$116</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Random Nearest Neighbour</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Time</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent4"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$117:$C$121</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>22 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>52 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>144 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>280 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>535 Point</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$G$117:$G$121</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-26D6-4211-8B4D-CFFC194212BC}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="365130440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365946360"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="365946360"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="365130440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Time for Different Point Sizes</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$H$115:$H$116</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>Hybrid Nearest Neighbour</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Time</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet1!$C$117:$C$121</c:f>
+              <c:strCache>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>22 Point</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>52 Point</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>144 Point</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>280 Point</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>535 Point</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$H$117:$H$121</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>15.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>115.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4306.3999999999996</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58941</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>708026.3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7893-49E3-A688-CCFBBA5D2149}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="400596352"/>
+        <c:axId val="400596680"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredBarSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$115:$I$116</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="2"/>
+                      <c:pt idx="0">
+                        <c:v>Hybrid Nearest Neighbour</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>Time</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:solidFill>
+                    <a:schemeClr val="accent2"/>
+                  </a:solidFill>
+                  <a:ln>
+                    <a:noFill/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:invertIfNegative val="0"/>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$C$117:$C$121</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="5"/>
+                      <c:pt idx="0">
+                        <c:v>22 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>52 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>144 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>280 Point</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>535 Point</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>Sheet1!$I$117:$I$121</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="5"/>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000001-7893-49E3-A688-CCFBBA5D2149}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredBarSeries>
+          </c:ext>
+        </c:extLst>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="400596352"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400596680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="400596680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="400596352"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -756,6 +1946,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1064,6 +2255,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1372,6 +2564,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1705,6 +2898,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2029,6 +3223,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2415,6 +3610,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2753,6 +3949,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3086,6 +4283,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3461,6 +4659,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -4789,6 +6067,1014 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style11.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style12.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
@@ -9153,6 +11439,66 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>126</xdr:row>
+      <xdr:rowOff>52387</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>111</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>125</xdr:row>
+      <xdr:rowOff>147637</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -9232,23 +11578,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -9284,23 +11613,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -9453,10 +11765,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:I113"/>
+  <dimension ref="C1:I121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C34" workbookViewId="0">
-      <selection activeCell="R113" sqref="R113"/>
+    <sheetView tabSelected="1" topLeftCell="F109" workbookViewId="0">
+      <selection activeCell="C126" sqref="C126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9773,21 +12085,21 @@
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="str">
-        <f>C1</f>
+        <f>$C$1</f>
         <v>Ulysses 22</v>
       </c>
       <c r="D17" s="2">
-        <f>AVERAGE(D4:D13)</f>
+        <f>AVERAGE($D$4:$D$13)</f>
         <v>0</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2">
-        <f>AVERAGE(F4:F13)</f>
+        <f>AVERAGE($F$4:$F$13)</f>
         <v>12.4</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2">
-        <f>AVERAGE(H4:H13)</f>
+        <f>AVERAGE($H$4:$H$13)</f>
         <v>15.5</v>
       </c>
       <c r="I17" s="2"/>
@@ -10149,21 +12461,21 @@
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" t="str">
-        <f>C24</f>
+        <f>$C$24</f>
         <v>Berlin 52</v>
       </c>
       <c r="D40" s="2">
-        <f>AVERAGE(D27:D36)</f>
+        <f>AVERAGE($D$27:$D$36)</f>
         <v>10.8</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2">
-        <f>AVERAGE(F27:F36)</f>
+        <f>AVERAGE($F$27:$F$36)</f>
         <v>18.7</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2">
-        <f>AVERAGE(H27:H36)</f>
+        <f>AVERAGE($H$27:$H$36)</f>
         <v>115.7</v>
       </c>
       <c r="I40" s="2"/>
@@ -10525,21 +12837,21 @@
     </row>
     <row r="63" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C63" t="str">
-        <f>C47</f>
+        <f>$C$47</f>
         <v>pr144</v>
       </c>
       <c r="D63" s="2">
-        <f>AVERAGE(D50:D59)</f>
+        <f>AVERAGE($D$50:$D$59)</f>
         <v>15.6</v>
       </c>
       <c r="E63" s="2"/>
       <c r="F63" s="2">
-        <f>AVERAGE(F50:F59)</f>
+        <f>AVERAGE($F$50:$F$59)</f>
         <v>17.399999999999999</v>
       </c>
       <c r="G63" s="2"/>
       <c r="H63" s="2">
-        <f>AVERAGE(H50:H59)</f>
+        <f>AVERAGE($H$50:$H$59)</f>
         <v>4306.3999999999996</v>
       </c>
       <c r="I63" s="2"/>
@@ -10901,21 +13213,21 @@
     </row>
     <row r="86" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C86" t="str">
-        <f>C70</f>
+        <f>$C$70</f>
         <v>a280</v>
       </c>
       <c r="D86" s="2">
-        <f>AVERAGE(D73:D82)</f>
+        <f>AVERAGE($D$73:$D$82)</f>
         <v>15.6</v>
       </c>
       <c r="E86" s="2"/>
       <c r="F86" s="2">
-        <f>AVERAGE(F73:F82)</f>
+        <f>AVERAGE($F$73:$F$82)</f>
         <v>33</v>
       </c>
       <c r="G86" s="2"/>
       <c r="H86" s="2">
-        <f>AVERAGE(H73:H82)</f>
+        <f>AVERAGE($H$73:$H$82)</f>
         <v>58941</v>
       </c>
       <c r="I86" s="2"/>
@@ -11277,21 +13589,21 @@
     </row>
     <row r="109" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C109" t="str">
-        <f>C93</f>
+        <f>$C$93</f>
         <v>ali535</v>
       </c>
       <c r="D109" s="2">
-        <f>AVERAGE(D96:D105)</f>
+        <f>AVERAGE($D$96:$D$105)</f>
         <v>16.7</v>
       </c>
       <c r="E109" s="2"/>
       <c r="F109" s="2">
-        <f>AVERAGE(F96:F105)</f>
+        <f>AVERAGE($F$96:$F$105)</f>
         <v>62.3</v>
       </c>
       <c r="G109" s="2"/>
       <c r="H109" s="2">
-        <f>AVERAGE(H96:H105)</f>
+        <f>AVERAGE($H$96:$H$105)</f>
         <v>708026.3</v>
       </c>
       <c r="I109" s="2"/>
@@ -11345,51 +13657,195 @@
       </c>
       <c r="I113" s="2"/>
     </row>
+    <row r="115" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D115" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E115" s="2"/>
+      <c r="F115" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="G115" s="2"/>
+      <c r="H115" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I115" s="2"/>
+    </row>
+    <row r="116" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="D116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I116" s="2"/>
+    </row>
+    <row r="117" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C117" t="s">
+        <v>11</v>
+      </c>
+      <c r="D117" s="2">
+        <f>AVERAGE($D$4:$D$13)</f>
+        <v>0</v>
+      </c>
+      <c r="E117" s="2"/>
+      <c r="F117" s="2">
+        <f>AVERAGE($F$4:$F$13)</f>
+        <v>12.4</v>
+      </c>
+      <c r="G117" s="2"/>
+      <c r="H117" s="2">
+        <f>AVERAGE($H$4:$H$13)</f>
+        <v>15.5</v>
+      </c>
+      <c r="I117" s="2"/>
+    </row>
+    <row r="118" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C118" t="s">
+        <v>12</v>
+      </c>
+      <c r="D118" s="2">
+        <f>AVERAGE($D$27:$D$36)</f>
+        <v>10.8</v>
+      </c>
+      <c r="E118" s="2"/>
+      <c r="F118" s="2">
+        <f>AVERAGE($F$27:$F$36)</f>
+        <v>18.7</v>
+      </c>
+      <c r="G118" s="2"/>
+      <c r="H118" s="2">
+        <f>AVERAGE($H$27:$H$36)</f>
+        <v>115.7</v>
+      </c>
+      <c r="I118" s="2"/>
+    </row>
+    <row r="119" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C119" t="s">
+        <v>13</v>
+      </c>
+      <c r="D119" s="2">
+        <f>AVERAGE($D$50:$D$59)</f>
+        <v>15.6</v>
+      </c>
+      <c r="E119" s="2"/>
+      <c r="F119" s="2">
+        <f>AVERAGE($F$50:$F$59)</f>
+        <v>17.399999999999999</v>
+      </c>
+      <c r="G119" s="2"/>
+      <c r="H119" s="2">
+        <f>AVERAGE($H$50:$H$59)</f>
+        <v>4306.3999999999996</v>
+      </c>
+      <c r="I119" s="2"/>
+    </row>
+    <row r="120" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C120" t="s">
+        <v>14</v>
+      </c>
+      <c r="D120" s="2">
+        <f>AVERAGE($D$73:$D$82)</f>
+        <v>15.6</v>
+      </c>
+      <c r="E120" s="2"/>
+      <c r="F120" s="2">
+        <f>AVERAGE($F$73:$F$82)</f>
+        <v>33</v>
+      </c>
+      <c r="G120" s="2"/>
+      <c r="H120" s="2">
+        <f>AVERAGE($H$73:$H$82)</f>
+        <v>58941</v>
+      </c>
+      <c r="I120" s="2"/>
+    </row>
+    <row r="121" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C121" t="s">
+        <v>15</v>
+      </c>
+      <c r="D121" s="2">
+        <f>AVERAGE($D$96:$D$105)</f>
+        <v>16.7</v>
+      </c>
+      <c r="E121" s="2"/>
+      <c r="F121" s="2">
+        <f>AVERAGE($F$96:$F$105)</f>
+        <v>62.3</v>
+      </c>
+      <c r="G121" s="2"/>
+      <c r="H121" s="2">
+        <f>AVERAGE($H$96:$H$105)</f>
+        <v>708026.3</v>
+      </c>
+      <c r="I121" s="2"/>
+    </row>
   </sheetData>
-  <mergeCells count="110">
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="H2:I2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="C1:I1"/>
-    <mergeCell ref="C93:I93"/>
-    <mergeCell ref="D94:E94"/>
-    <mergeCell ref="F94:G94"/>
-    <mergeCell ref="H94:I94"/>
-    <mergeCell ref="C47:I47"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="F48:G48"/>
-    <mergeCell ref="H48:I48"/>
-    <mergeCell ref="C70:I70"/>
-    <mergeCell ref="D71:E71"/>
-    <mergeCell ref="F71:G71"/>
-    <mergeCell ref="H71:I71"/>
-    <mergeCell ref="F85:G85"/>
-    <mergeCell ref="H85:I85"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="F86:G86"/>
-    <mergeCell ref="F108:G108"/>
-    <mergeCell ref="F109:G109"/>
-    <mergeCell ref="H108:I108"/>
-    <mergeCell ref="H109:I109"/>
-    <mergeCell ref="D109:E109"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D112:E112"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="F25:G25"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="D111:E111"/>
-    <mergeCell ref="F111:G111"/>
-    <mergeCell ref="H111:I111"/>
-    <mergeCell ref="D61:E61"/>
-    <mergeCell ref="F61:G61"/>
-    <mergeCell ref="H61:I61"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="F38:G38"/>
-    <mergeCell ref="H38:I38"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="F42:G42"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="D85:E85"/>
+  <mergeCells count="131">
+    <mergeCell ref="D120:E120"/>
+    <mergeCell ref="F120:G120"/>
+    <mergeCell ref="H120:I120"/>
+    <mergeCell ref="D121:E121"/>
+    <mergeCell ref="F121:G121"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="D118:E118"/>
+    <mergeCell ref="F118:G118"/>
+    <mergeCell ref="H118:I118"/>
+    <mergeCell ref="D115:E115"/>
+    <mergeCell ref="F115:G115"/>
+    <mergeCell ref="H115:I115"/>
+    <mergeCell ref="D119:E119"/>
+    <mergeCell ref="F119:G119"/>
+    <mergeCell ref="H119:I119"/>
+    <mergeCell ref="H43:I43"/>
+    <mergeCell ref="D44:E44"/>
+    <mergeCell ref="F44:G44"/>
+    <mergeCell ref="H44:I44"/>
+    <mergeCell ref="D116:E116"/>
+    <mergeCell ref="F116:G116"/>
+    <mergeCell ref="H116:I116"/>
+    <mergeCell ref="D117:E117"/>
+    <mergeCell ref="F117:G117"/>
+    <mergeCell ref="H117:I117"/>
+    <mergeCell ref="D67:E67"/>
+    <mergeCell ref="H86:I86"/>
+    <mergeCell ref="D88:E88"/>
+    <mergeCell ref="F88:G88"/>
+    <mergeCell ref="H88:I88"/>
+    <mergeCell ref="D89:E89"/>
+    <mergeCell ref="F89:G89"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="F20:G20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="D21:E21"/>
+    <mergeCell ref="F21:G21"/>
+    <mergeCell ref="H21:I21"/>
+    <mergeCell ref="F67:G67"/>
+    <mergeCell ref="H67:I67"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="F39:G39"/>
+    <mergeCell ref="H39:I39"/>
+    <mergeCell ref="D40:E40"/>
+    <mergeCell ref="F40:G40"/>
+    <mergeCell ref="H40:I40"/>
+    <mergeCell ref="D43:E43"/>
+    <mergeCell ref="F43:G43"/>
+    <mergeCell ref="H62:I62"/>
+    <mergeCell ref="D63:E63"/>
+    <mergeCell ref="F63:G63"/>
+    <mergeCell ref="H63:I63"/>
+    <mergeCell ref="D65:E65"/>
+    <mergeCell ref="F65:G65"/>
+    <mergeCell ref="H65:I65"/>
+    <mergeCell ref="D66:E66"/>
+    <mergeCell ref="F66:G66"/>
+    <mergeCell ref="H66:I66"/>
     <mergeCell ref="D113:E113"/>
     <mergeCell ref="F113:G113"/>
     <mergeCell ref="F112:G112"/>
@@ -11414,49 +13870,54 @@
     <mergeCell ref="H107:I107"/>
     <mergeCell ref="F107:G107"/>
     <mergeCell ref="D107:E107"/>
+    <mergeCell ref="F108:G108"/>
+    <mergeCell ref="F109:G109"/>
+    <mergeCell ref="H108:I108"/>
+    <mergeCell ref="H109:I109"/>
+    <mergeCell ref="D109:E109"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D112:E112"/>
+    <mergeCell ref="D25:E25"/>
+    <mergeCell ref="F25:G25"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="D111:E111"/>
+    <mergeCell ref="F111:G111"/>
+    <mergeCell ref="H111:I111"/>
+    <mergeCell ref="D61:E61"/>
+    <mergeCell ref="F61:G61"/>
+    <mergeCell ref="H61:I61"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="F38:G38"/>
+    <mergeCell ref="H38:I38"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="F42:G42"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="D85:E85"/>
     <mergeCell ref="D90:E90"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="H2:I2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="C1:I1"/>
+    <mergeCell ref="C93:I93"/>
+    <mergeCell ref="D94:E94"/>
+    <mergeCell ref="F94:G94"/>
+    <mergeCell ref="H94:I94"/>
+    <mergeCell ref="C47:I47"/>
+    <mergeCell ref="D48:E48"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="H48:I48"/>
+    <mergeCell ref="C70:I70"/>
+    <mergeCell ref="D71:E71"/>
+    <mergeCell ref="F71:G71"/>
+    <mergeCell ref="H71:I71"/>
+    <mergeCell ref="F85:G85"/>
+    <mergeCell ref="H85:I85"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="F86:G86"/>
     <mergeCell ref="F90:G90"/>
     <mergeCell ref="H90:I90"/>
     <mergeCell ref="D62:E62"/>
     <mergeCell ref="F62:G62"/>
-    <mergeCell ref="H62:I62"/>
-    <mergeCell ref="D63:E63"/>
-    <mergeCell ref="F63:G63"/>
-    <mergeCell ref="H63:I63"/>
-    <mergeCell ref="D65:E65"/>
-    <mergeCell ref="F65:G65"/>
-    <mergeCell ref="H65:I65"/>
-    <mergeCell ref="D66:E66"/>
-    <mergeCell ref="F66:G66"/>
-    <mergeCell ref="H66:I66"/>
-    <mergeCell ref="D67:E67"/>
-    <mergeCell ref="H86:I86"/>
-    <mergeCell ref="D88:E88"/>
-    <mergeCell ref="F88:G88"/>
-    <mergeCell ref="H88:I88"/>
-    <mergeCell ref="D89:E89"/>
-    <mergeCell ref="F89:G89"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="F20:G20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="F21:G21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="F67:G67"/>
-    <mergeCell ref="H67:I67"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="F39:G39"/>
-    <mergeCell ref="H39:I39"/>
-    <mergeCell ref="D40:E40"/>
-    <mergeCell ref="F40:G40"/>
-    <mergeCell ref="H40:I40"/>
-    <mergeCell ref="D43:E43"/>
-    <mergeCell ref="F43:G43"/>
-    <mergeCell ref="H43:I43"/>
-    <mergeCell ref="D44:E44"/>
-    <mergeCell ref="F44:G44"/>
-    <mergeCell ref="H44:I44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>